<commit_message>
[PHOENIX-5853] UI : Checking WCMS Module Automationin UAT  according to the latest dump
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="178">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">addressOne</t>
   </si>
   <si>
-    <t xml:space="preserve">abass nagar</t>
+    <t xml:space="preserve">Auto Nagar</t>
   </si>
   <si>
     <t xml:space="preserve">Zone1</t>
@@ -226,10 +226,10 @@
     <t xml:space="preserve">1st floor</t>
   </si>
   <si>
-    <t xml:space="preserve">cements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residencial</t>
+    <t xml:space="preserve">Huts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residence</t>
   </si>
   <si>
     <t xml:space="preserve">FirmName</t>
@@ -332,9 +332,6 @@
   </si>
   <si>
     <t xml:space="preserve">HUTSSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residence</t>
   </si>
   <si>
     <t xml:space="preserve">NA</t>
@@ -793,13 +790,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,21 +866,20 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.0612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.9081632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,16 +940,16 @@
         <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="H2" s="5" t="n">
         <v>42319</v>
@@ -971,7 +967,7 @@
         <v>20</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N2" s="5" t="n">
         <v>42358</v>
@@ -1004,11 +1000,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,21 +1012,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1057,10 +1053,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1068,21 +1065,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1109,10 +1106,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1120,15 +1116,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1156,25 +1152,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7704081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.25"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.9795918367347"/>
     <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1182,69 +1178,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>30</v>
@@ -1253,28 +1249,28 @@
         <v>20</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="N2" s="6" t="n">
         <v>121</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P2" s="6" t="n">
         <v>500000</v>
@@ -1308,81 +1304,81 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="15" t="n">
         <v>1016063818</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>142</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>144</v>
-      </c>
       <c r="C4" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="C5" s="0" t="s">
         <v>146</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>148</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>150</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1411,25 +1407,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>153</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1456,39 +1452,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>156</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>160</v>
-      </c>
       <c r="D2" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1514,45 +1510,48 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>168</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>170</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>171</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>111</v>
@@ -1567,16 +1566,16 @@
         <v>300</v>
       </c>
       <c r="G2" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>174</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1603,12 +1602,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1619,7 +1619,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
@@ -1881,10 +1881,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1016094460</v>
@@ -2171,13 +2171,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.0204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="40.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="40.0918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2229,19 +2229,19 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2314,8 +2314,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2401,9 +2401,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.0204081632653"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2460,32 +2460,32 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.8673469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="34.0204081632653"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2606,11 +2606,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2665,11 +2665,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="41.7142857142857"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.7959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2719,11 +2718,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-7804] Modified the changes of create property
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -262,7 +262,7 @@
     <t xml:space="preserve">43051</t>
   </si>
   <si>
-    <t xml:space="preserve">20/12/2016</t>
+    <t xml:space="preserve">09/01/2018</t>
   </si>
   <si>
     <t xml:space="preserve">assessmentAdditionProperty</t>
@@ -586,7 +586,7 @@
     <numFmt numFmtId="168" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="169" formatCode="HH:MM\ AM/PM"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -621,6 +621,12 @@
       <name val="Menlo"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -683,7 +689,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -708,7 +714,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -728,15 +742,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -790,13 +804,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -872,14 +885,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.9081632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -960,10 +974,10 @@
       <c r="J2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="8" t="n">
+      <c r="K2" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="8" t="n">
+      <c r="L2" s="10" t="n">
         <v>20</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -1000,11 +1014,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1053,11 +1066,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1106,9 +1119,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1152,35 +1166,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.5"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.7091836734694"/>
     <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>113</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1207,7 +1220,7 @@
       <c r="K1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="11" t="s">
         <v>122</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -1242,10 +1255,10 @@
       <c r="E2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="G2" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -1266,16 +1279,16 @@
       <c r="M2" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="N2" s="6" t="n">
+      <c r="N2" s="7" t="n">
         <v>121</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="P2" s="6" t="n">
+      <c r="P2" s="7" t="n">
         <v>500000</v>
       </c>
-      <c r="Q2" s="6" t="n">
+      <c r="Q2" s="7" t="n">
         <v>900000</v>
       </c>
     </row>
@@ -1304,28 +1317,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="15" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="15" t="n">
+      <c r="B2" s="17" t="n">
         <v>1016063818</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -1333,10 +1346,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="17" t="s">
         <v>141</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -1344,10 +1357,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="17" t="s">
         <v>143</v>
       </c>
       <c r="C4" s="0" t="s">
@@ -1355,10 +1368,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="17" t="s">
         <v>145</v>
       </c>
       <c r="C5" s="0" t="s">
@@ -1369,7 +1382,7 @@
       <c r="A6" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="18" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1377,7 +1390,7 @@
       <c r="A7" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="18" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1407,16 +1420,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1424,7 +1437,7 @@
       <c r="A2" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1452,18 +1465,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="19" t="s">
         <v>154</v>
       </c>
       <c r="C1" s="0" t="s">
@@ -1477,10 +1490,10 @@
       <c r="A2" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="21" t="s">
         <v>159</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -1511,14 +1524,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>160</v>
       </c>
       <c r="C1" s="0" t="s">
@@ -1550,7 +1563,7 @@
       <c r="A2" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>170</v>
       </c>
       <c r="C2" s="0" t="n">
@@ -1602,13 +1615,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2171,13 +2184,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2234,14 +2246,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2314,8 +2325,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2401,9 +2411,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2460,32 +2469,30 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2558,10 +2565,10 @@
         <v>8</v>
       </c>
       <c r="H2" s="5" t="n">
-        <v>42835</v>
-      </c>
-      <c r="I2" s="5" t="n">
-        <v>42866</v>
+        <v>43110</v>
+      </c>
+      <c r="I2" s="6" t="n">
+        <v>43110</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>66</v>
@@ -2575,8 +2582,8 @@
       <c r="M2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="N2" s="5" t="n">
-        <v>42358</v>
+      <c r="N2" s="6" t="n">
+        <v>43110</v>
       </c>
       <c r="O2" s="1" t="n">
         <v>30</v>
@@ -2600,17 +2607,17 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2634,10 +2641,10 @@
       <c r="B2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2665,17 +2672,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.7959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="41.1734693877551"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="40.6326530612245"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2718,11 +2726,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-7813] modified search property changes
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="176">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -463,28 +463,22 @@
     <t xml:space="preserve">searchWithMobileNumber</t>
   </si>
   <si>
-    <t xml:space="preserve">0000161311</t>
+    <t xml:space="preserve">2222223444</t>
   </si>
   <si>
     <t xml:space="preserve">searchWithDoorNumber</t>
   </si>
   <si>
-    <t xml:space="preserve">87/1110-9-c</t>
-  </si>
-  <si>
     <t xml:space="preserve">searchWithZoneAndWardNumber</t>
   </si>
   <si>
-    <t xml:space="preserve">Zone-15;Revenue Ward No  87</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87/1110-9-c;C. Naga Sailaja W/o R. Satish Kumar</t>
+    <t xml:space="preserve">Zone1;Revenue Ward No 2</t>
   </si>
   <si>
     <t xml:space="preserve">searchWithOwnerName</t>
   </si>
   <si>
-    <t xml:space="preserve">revenue colony;C. Naga Sailaja W/o R. Satish Kumar</t>
+    <t xml:space="preserve">Krishna Nagar;Peram Subramanyam</t>
   </si>
   <si>
     <t xml:space="preserve">searchByDemand</t>
@@ -586,7 +580,7 @@
     <numFmt numFmtId="168" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="169" formatCode="HH:MM\ AM/PM"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -621,12 +615,6 @@
       <name val="Menlo"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -689,7 +677,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -714,15 +702,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -742,15 +722,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -799,17 +779,18 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -885,15 +866,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,10 +955,10 @@
       <c r="J2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="10" t="n">
+      <c r="K2" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="10" t="n">
+      <c r="L2" s="8" t="n">
         <v>20</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -1014,10 +995,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,11 +1048,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1119,10 +1100,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1166,34 +1147,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.0918367346939"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.1683673469388"/>
     <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>113</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1220,7 +1202,7 @@
       <c r="K1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="9" t="s">
         <v>122</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -1255,10 +1237,10 @@
       <c r="E2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="G2" s="7" t="n">
+      <c r="G2" s="6" t="n">
         <v>20</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -1279,16 +1261,16 @@
       <c r="M2" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="N2" s="7" t="n">
+      <c r="N2" s="6" t="n">
         <v>121</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="P2" s="7" t="n">
+      <c r="P2" s="6" t="n">
         <v>500000</v>
       </c>
-      <c r="Q2" s="7" t="n">
+      <c r="Q2" s="6" t="n">
         <v>900000</v>
       </c>
     </row>
@@ -1311,87 +1293,93 @@
   </sheetPr>
   <dimension ref="A1:C65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="33.4795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="17" t="n">
+      <c r="B2" s="15" t="n">
         <v>1016063818</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>141</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>143</v>
+      <c r="B4" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="C5" s="0" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>148</v>
+        <v>145</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>150</v>
+        <v>147</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1420,25 +1408,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>151</v>
+      <c r="B1" s="14" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>153</v>
+        <v>150</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1465,36 +1453,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>157</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>159</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>130</v>
@@ -1523,48 +1511,45 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>170</v>
+        <v>167</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>111</v>
@@ -1579,16 +1564,16 @@
         <v>300</v>
       </c>
       <c r="G2" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>172</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1615,13 +1600,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1632,7 +1616,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
@@ -1894,10 +1878,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1016094460</v>
@@ -2184,12 +2168,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="39.6887755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.7448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2241,18 +2226,19 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2325,7 +2311,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2411,8 +2398,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,24 +2463,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2567,7 +2557,7 @@
       <c r="H2" s="5" t="n">
         <v>43110</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="5" t="n">
         <v>43110</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -2582,7 +2572,7 @@
       <c r="M2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="N2" s="6" t="n">
+      <c r="N2" s="5" t="n">
         <v>43110</v>
       </c>
       <c r="O2" s="1" t="n">
@@ -2607,17 +2597,17 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2641,10 +2631,10 @@
       <c r="B2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2672,18 +2662,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="40.6326530612245"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2726,10 +2716,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-7817] modified the changes in addition of property screen
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="175">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -329,9 +329,6 @@
   </si>
   <si>
     <t xml:space="preserve">2nd Floor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HUTSSS</t>
   </si>
   <si>
     <t xml:space="preserve">NA</t>
@@ -784,13 +781,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -858,23 +855,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.5765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,19 +928,19 @@
         <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="H2" s="5" t="n">
         <v>42319</v>
@@ -962,7 +958,7 @@
         <v>20</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N2" s="5" t="n">
         <v>42358</v>
@@ -971,6 +967,8 @@
         <v>50</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -995,11 +993,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.25"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,21 +1005,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1048,10 +1046,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1059,21 +1058,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1100,10 +1099,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1111,15 +1109,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1147,25 +1145,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.9591836734694"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="18.8979591836735"/>
     <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1173,69 +1171,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>30</v>
@@ -1244,28 +1242,28 @@
         <v>20</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="N2" s="6" t="n">
         <v>121</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P2" s="6" t="n">
         <v>500000</v>
@@ -1293,93 +1291,93 @@
   </sheetPr>
   <dimension ref="A1:C65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>136</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="15" t="n">
         <v>1016063818</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>141</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>144</v>
-      </c>
       <c r="C5" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>146</v>
-      </c>
       <c r="C6" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>148</v>
-      </c>
       <c r="C7" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1408,25 +1406,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1453,39 +1451,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>153</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>157</v>
-      </c>
       <c r="D2" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1511,45 +1509,48 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>165</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>167</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>168</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>111</v>
@@ -1564,16 +1565,16 @@
         <v>300</v>
       </c>
       <c r="G2" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>171</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1600,12 +1601,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,7 +1618,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
@@ -1878,10 +1880,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1016094460</v>
@@ -2168,13 +2170,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2231,14 +2233,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2311,8 +2313,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2398,9 +2400,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2463,26 +2465,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2603,11 +2605,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2662,11 +2664,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.6887755102041"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.280612244898"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2716,11 +2717,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-7860] modified changes in demolition of property
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -781,13 +781,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -857,20 +856,21 @@
   </sheetPr>
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.0357142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="40.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -993,11 +993,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,11 +1045,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1099,9 +1098,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1145,25 +1145,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.8265306122449"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="18.6275510204082"/>
     <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1297,10 +1296,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,9 +1405,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1451,11 +1450,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1504,13 +1503,13 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1562,7 +1561,7 @@
         <v>200</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>168</v>
@@ -1601,13 +1600,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2170,13 +2169,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.2040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.6632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2233,14 +2231,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2313,8 +2310,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2400,9 +2396,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2465,26 +2460,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2605,11 +2598,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2664,10 +2657,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.280612244898"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="38.7448979591837"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2717,11 +2711,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>